<commit_message>
Added save_arrhenius and import_arrhenius functions + created analysis notebook for arrhenius comparison
These functions allow to save and then read the arrhenius info such as the actual arrhenius plot data and the trap parameters (Ea, sigma and errors).
This will allow to simplify further analysis of the arrhenius plots in order to compare different samples.

I also started to create the notebook that
compares arrhenius plots of all samples, with statistical analysis of the data.
</commit_message>
<xml_diff>
--- a/Data/defects_in_MAPbBr3/sample_info.xlsx
+++ b/Data/defects_in_MAPbBr3/sample_info.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giovanni/Documents/Python_Libraries/mylib/Data/defects_in_MAPbBr3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{075981D2-862E-154A-AD37-D9AF768D6683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B0E71DC-C656-8B48-BF27-60D8BF5DF386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{C26AC50F-A531-6740-AF76-4A280DDFF701}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
   <si>
     <t>Sample name</t>
   </si>
@@ -70,9 +70,6 @@
     <t>T max (K)</t>
   </si>
   <si>
-    <t>Light soure current (mA)</t>
-  </si>
-  <si>
     <t>Cr</t>
   </si>
   <si>
@@ -98,6 +95,15 @@
   </si>
   <si>
     <t>Light intensity (W/cm2)</t>
+  </si>
+  <si>
+    <t>T range (K)</t>
+  </si>
+  <si>
+    <t>Light source current (mA)</t>
+  </si>
+  <si>
+    <t>Sample age (days)</t>
   </si>
 </sst>
 </file>
@@ -485,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E561E7DD-3721-9549-879B-F206EB3A7F40}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:Q8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="116" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -509,7 +515,7 @@
     <col min="14" max="14" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -535,16 +541,16 @@
         <v>7</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>10</v>
@@ -555,8 +561,14 @@
       <c r="O1" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="P1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1013</v>
       </c>
@@ -567,19 +579,19 @@
         <v>44343</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" t="s">
-        <v>15</v>
-      </c>
       <c r="I2" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J2">
         <v>460</v>
@@ -596,8 +608,16 @@
       <c r="O2">
         <v>5</v>
       </c>
+      <c r="P2">
+        <f>C2-B2</f>
+        <v>12</v>
+      </c>
+      <c r="Q2">
+        <f>N2-M2</f>
+        <v>270</v>
+      </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1113</v>
       </c>
@@ -608,19 +628,19 @@
         <v>44384</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
         <v>13</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>14</v>
       </c>
-      <c r="H3" t="s">
-        <v>15</v>
-      </c>
       <c r="I3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J3">
         <v>475</v>
@@ -637,8 +657,16 @@
       <c r="O3">
         <v>5</v>
       </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P5" si="0">C3-B3</f>
+        <v>30</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q5" si="1">N3-M3</f>
+        <v>222</v>
+      </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1212</v>
       </c>
@@ -649,22 +677,22 @@
         <v>44404</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
         <v>13</v>
-      </c>
-      <c r="F4" t="s">
-        <v>14</v>
       </c>
       <c r="G4">
         <v>8</v>
       </c>
       <c r="H4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J4">
         <v>475</v>
@@ -681,8 +709,16 @@
       <c r="O4">
         <v>5</v>
       </c>
+      <c r="P4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="1"/>
+        <v>180</v>
+      </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1213</v>
       </c>
@@ -693,22 +729,22 @@
         <v>44411</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
         <v>13</v>
-      </c>
-      <c r="F5" t="s">
-        <v>14</v>
       </c>
       <c r="G5">
         <v>8</v>
       </c>
       <c r="H5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J5">
         <v>475</v>
@@ -725,18 +761,26 @@
       <c r="O5">
         <v>5</v>
       </c>
+      <c r="P5">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="1"/>
+        <v>180</v>
+      </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1411</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1311</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1312</v>
       </c>

</xml_diff>

<commit_message>
Update arrhenius plot excel file
changed bias from +- to just 5V
</commit_message>
<xml_diff>
--- a/Data/defects_in_MAPbBr3/sample_info.xlsx
+++ b/Data/defects_in_MAPbBr3/sample_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinafoschi/Documents/GitHub/mylib/Data/defects_in_MAPbBr3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3121E91-138C-904F-816B-E0093010E188}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B9E3023-6E3A-0E44-B0C2-F92BCB93540A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="1080" windowWidth="25600" windowHeight="15540" xr2:uid="{C26AC50F-A531-6740-AF76-4A280DDFF701}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="24">
   <si>
     <t>Sample name</t>
   </si>
@@ -106,9 +106,6 @@
   </si>
   <si>
     <t>Sample age (days)</t>
-  </si>
-  <si>
-    <t>±5</t>
   </si>
 </sst>
 </file>
@@ -499,7 +496,7 @@
   <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -809,8 +806,8 @@
       <c r="F9" t="s">
         <v>13</v>
       </c>
-      <c r="G9" t="s">
-        <v>24</v>
+      <c r="G9">
+        <v>5</v>
       </c>
       <c r="H9" t="s">
         <v>14</v>
@@ -859,8 +856,8 @@
       <c r="F10" t="s">
         <v>13</v>
       </c>
-      <c r="G10" t="s">
-        <v>24</v>
+      <c r="G10">
+        <v>5</v>
       </c>
       <c r="H10" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
updated data and analysis on arrhenius plots
</commit_message>
<xml_diff>
--- a/Data/defects_in_MAPbBr3/sample_info.xlsx
+++ b/Data/defects_in_MAPbBr3/sample_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giovanni/Documents/Python_Libraries/mylib/Data/defects_in_MAPbBr3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE583D93-A4AB-264D-AD2E-FE6CF4DAFE30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{840749FB-555B-6745-A188-05E46221E68D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{C26AC50F-A531-6740-AF76-4A280DDFF701}"/>
   </bookViews>
@@ -429,7 +429,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>